<commit_message>
added checking for property in file
</commit_message>
<xml_diff>
--- a/properties_output.xlsx
+++ b/properties_output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="57">
   <si>
     <t>A</t>
   </si>
@@ -55,72 +55,87 @@
     <t>Contact Name</t>
   </si>
   <si>
-    <t>CARL HOLLISTER</t>
-  </si>
-  <si>
-    <t>MICHAEL PIHAKIS</t>
-  </si>
-  <si>
-    <t>CHRIST COUMANIS</t>
-  </si>
-  <si>
-    <t>ANGELO KOSTARIDES</t>
-  </si>
-  <si>
-    <t>ANGELA MAGRAMES</t>
-  </si>
-  <si>
-    <t>JOHN GROSSOMANIDES</t>
-  </si>
-  <si>
-    <t>JOHN MILLER</t>
-  </si>
-  <si>
-    <t>PETER NASSOS</t>
-  </si>
-  <si>
-    <t>JOHN ZOURZOUKIS</t>
-  </si>
-  <si>
-    <t>S CHRISTY KARTHAN</t>
-  </si>
-  <si>
-    <t>IKE GULAS</t>
-  </si>
-  <si>
-    <t>JIMMY MAKRIS</t>
-  </si>
-  <si>
-    <t>PANOS NIARCHOS</t>
+    <t>Albert Dudley</t>
+  </si>
+  <si>
+    <t>Benjamin Jones</t>
+  </si>
+  <si>
+    <t>D Snell</t>
+  </si>
+  <si>
+    <t>Andryna Kuzmicic</t>
+  </si>
+  <si>
+    <t>Paul Gunn</t>
+  </si>
+  <si>
+    <t>Marie Hollis</t>
+  </si>
+  <si>
+    <t>Carlos Coates</t>
+  </si>
+  <si>
+    <t>Cheri L Blair</t>
+  </si>
+  <si>
+    <t>Mitzi Johnson</t>
+  </si>
+  <si>
+    <t>Rev Don Koepke</t>
+  </si>
+  <si>
+    <t>Anita McCrimon</t>
+  </si>
+  <si>
+    <t>Robert Covington</t>
+  </si>
+  <si>
+    <t>Martin T Laurent</t>
+  </si>
+  <si>
+    <t>Jean Enock Berus</t>
+  </si>
+  <si>
+    <t>Robert J Chillison II</t>
   </si>
   <si>
     <t>Owner Organization Name</t>
   </si>
   <si>
-    <t>AHEPA 23 II, Inc.</t>
+    <t>HUNTSVILLE ADVENTIST APARTMENTS, INC.</t>
   </si>
   <si>
     <t>Phone</t>
   </si>
   <si>
+    <t>SOUTH BAY RETIREMENT RESIDENCE</t>
+  </si>
+  <si>
     <t>Property Name</t>
   </si>
   <si>
-    <t>AHEPA 23-II APARTMENTS</t>
+    <t>HUNTSVILLE ADVENT APTS</t>
   </si>
   <si>
     <t>Email</t>
   </si>
   <si>
+    <t>South Bay Retirement Residence</t>
+  </si>
+  <si>
     <t>Project Category</t>
   </si>
   <si>
+    <t>Insured-Subsidized</t>
+  </si>
+  <si>
+    <t>Adress</t>
+  </si>
+  <si>
     <t>202/811</t>
   </si>
   <si>
-    <t>Adress</t>
-  </si>
-  <si>
     <t>Owner Company Type</t>
   </si>
   <si>
@@ -136,13 +151,19 @@
     <t>(Address) Line 1</t>
   </si>
   <si>
-    <t>285 Sylvest Drive</t>
+    <t>3409 NW VENONA AVE</t>
+  </si>
+  <si>
+    <t>1001 W CRESSEY ST</t>
   </si>
   <si>
     <t>(Address) City</t>
   </si>
   <si>
-    <t>MONTGOMERY</t>
+    <t>HUNTSVILLE</t>
+  </si>
+  <si>
+    <t>COMPTON</t>
   </si>
   <si>
     <t>(Address) State</t>
@@ -151,13 +172,19 @@
     <t>AL</t>
   </si>
   <si>
+    <t>CA</t>
+  </si>
+  <si>
     <t>(Address) Postal Code</t>
   </si>
   <si>
     <t>ProPublica Link</t>
   </si>
   <si>
-    <t>https://projects.propublica.org/nonprofits/organizations/631140959</t>
+    <t>https://projects.propublica.org/nonprofits/organizations/630878986</t>
+  </si>
+  <si>
+    <t>https://projects.propublica.org/nonprofits/organizations/954321266</t>
   </si>
 </sst>
 </file>
@@ -528,7 +555,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:K54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -574,66 +601,66 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="J2" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="K2" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:11">
       <c r="A3">
-        <v>800000130</v>
+        <v>800000304</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F3">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I3" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -641,16 +668,16 @@
         <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="E4" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -680,42 +707,111 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>53</v>
+      </c>
+      <c r="K10" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="11" spans="1:11">
-      <c r="A11" t="s">
-        <v>19</v>
+      <c r="A11">
+        <v>800000304</v>
+      </c>
+      <c r="B11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11">
+        <v>76</v>
+      </c>
+      <c r="G11" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="A12" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:11">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:11">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -723,72 +819,84 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F18" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G18" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H18" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I18" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="J18" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="K18" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:11">
       <c r="A19">
-        <v>800000130</v>
+        <v>800000304</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="F19">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="G19" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="H19" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I19" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:11">
       <c r="A20" t="s">
         <v>12</v>
       </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="21" spans="1:11">
       <c r="A21" t="s">
@@ -817,48 +925,364 @@
     </row>
     <row r="26" spans="1:11">
       <c r="A26" t="s">
-        <v>18</v>
+        <v>11</v>
+      </c>
+      <c r="B26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D26" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>43</v>
+      </c>
+      <c r="G26" t="s">
+        <v>44</v>
+      </c>
+      <c r="H26" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" t="s">
+        <v>50</v>
+      </c>
+      <c r="J26" t="s">
+        <v>53</v>
+      </c>
+      <c r="K26" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" t="s">
-        <v>19</v>
+      <c r="A27">
+        <v>800000304</v>
+      </c>
+      <c r="B27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" t="s">
+        <v>33</v>
+      </c>
+      <c r="D27" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" t="s">
+        <v>41</v>
+      </c>
+      <c r="F27">
+        <v>76</v>
+      </c>
+      <c r="G27" t="s">
+        <v>45</v>
+      </c>
+      <c r="H27" t="s">
+        <v>48</v>
+      </c>
+      <c r="I27" t="s">
+        <v>51</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" t="s">
-        <v>20</v>
+        <v>12</v>
+      </c>
+      <c r="B28" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="31" spans="1:11">
       <c r="A31" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:11">
       <c r="A32" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" t="s">
+        <v>32</v>
+      </c>
+      <c r="D34" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H34" t="s">
+        <v>47</v>
+      </c>
+      <c r="I34" t="s">
+        <v>50</v>
+      </c>
+      <c r="J34" t="s">
+        <v>53</v>
+      </c>
+      <c r="K34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35">
+        <v>800000067</v>
+      </c>
+      <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
+        <v>39</v>
+      </c>
+      <c r="E35" t="s">
+        <v>41</v>
+      </c>
+      <c r="F35">
+        <v>75</v>
+      </c>
+      <c r="G35" t="s">
+        <v>46</v>
+      </c>
+      <c r="H35" t="s">
+        <v>49</v>
+      </c>
+      <c r="I35" t="s">
+        <v>52</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" t="s">
+        <v>12</v>
+      </c>
+      <c r="B36" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" t="s">
+        <v>34</v>
+      </c>
+      <c r="D36" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" t="s">
+        <v>40</v>
+      </c>
+      <c r="F47" t="s">
+        <v>43</v>
+      </c>
+      <c r="G47" t="s">
+        <v>44</v>
+      </c>
+      <c r="H47" t="s">
+        <v>47</v>
+      </c>
+      <c r="I47" t="s">
+        <v>50</v>
+      </c>
+      <c r="J47" t="s">
+        <v>53</v>
+      </c>
+      <c r="K47" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48">
+        <v>800000304</v>
+      </c>
+      <c r="B48" t="s">
+        <v>29</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E48" t="s">
+        <v>41</v>
+      </c>
+      <c r="F48">
+        <v>76</v>
+      </c>
+      <c r="G48" t="s">
+        <v>45</v>
+      </c>
+      <c r="H48" t="s">
+        <v>48</v>
+      </c>
+      <c r="I48" t="s">
+        <v>51</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>12</v>
+      </c>
+      <c r="B49" t="s">
+        <v>30</v>
+      </c>
+      <c r="C49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" t="s">
+        <v>38</v>
+      </c>
+      <c r="E49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1"/>
-    <hyperlink ref="K19" r:id="rId2"/>
+    <hyperlink ref="K11" r:id="rId2"/>
+    <hyperlink ref="K19" r:id="rId3"/>
+    <hyperlink ref="K27" r:id="rId4"/>
+    <hyperlink ref="K35" r:id="rId5"/>
+    <hyperlink ref="K48" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>